<commit_message>
Market name on sheet
</commit_message>
<xml_diff>
--- a/excel_actualizado.xlsx
+++ b/excel_actualizado.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="VARIOS" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -460,7 +460,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>16699</v>
+        <v>15799</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -491,7 +491,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>13399</v>
+        <v>12199</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6899</v>
+        <v>6299</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9899</v>
+        <v>8999</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -584,7 +584,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>19299</v>
+        <v>17599</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -615,7 +615,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>11899</v>
+        <v>10799</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -646,7 +646,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>16299</v>
+        <v>14799</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>17199</v>
+        <v>15699</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -708,7 +708,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>17899</v>
+        <v>16299</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -739,7 +739,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>71399</v>
+        <v>64999</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -770,7 +770,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>22799</v>
+        <v>20799</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -801,7 +801,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>26599</v>
+        <v>24299</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -832,7 +832,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>25299</v>
+        <v>22999</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -863,7 +863,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>32799</v>
+        <v>29899</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -894,7 +894,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7099</v>
+        <v>6499</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5499</v>
+        <v>4999</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -956,7 +956,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>20299</v>
+        <v>18499</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>14499</v>
+        <v>13199</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>13899</v>
+        <v>12699</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>37599</v>
+        <v>34199</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>15599</v>
+        <v>14299</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>13199</v>
+        <v>11999</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>9099</v>
+        <v>8299</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>11299</v>
+        <v>10299</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>15499</v>
+        <v>14099</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>9999</v>
+        <v>9099</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>32199</v>
+        <v>29399</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>21799</v>
+        <v>19799</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>9399</v>
+        <v>8599</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>46199</v>
+        <v>42099</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>27399</v>
+        <v>24899</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>17399</v>
+        <v>15899</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>28099</v>
+        <v>25599</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>22499</v>
+        <v>20499</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>17799</v>
+        <v>16199</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>

</xml_diff>